<commit_message>
13 Jul 2016:  All HTTP Calls have proper, functioning erorr handlers
</commit_message>
<xml_diff>
--- a/coffeeAppIssuesLog.xlsx
+++ b/coffeeAppIssuesLog.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="19">
   <si>
     <t>Project:</t>
   </si>
@@ -56,12 +56,6 @@
     <t>All pages need to be styled</t>
   </si>
   <si>
-    <t>Callback Functions</t>
-  </si>
-  <si>
-    <t>All functions need to be reviewed for proper error handling.</t>
-  </si>
-  <si>
     <t>README.md</t>
   </si>
   <si>
@@ -81,6 +75,12 @@
   </si>
   <si>
     <t>real navigation links / hamburger</t>
+  </si>
+  <si>
+    <t>Update CB Functions / Error Handling / Front End</t>
+  </si>
+  <si>
+    <t>Closed</t>
   </si>
 </sst>
 </file>
@@ -599,10 +599,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E12"/>
+  <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0.2"/>
@@ -653,13 +653,10 @@
     </row>
     <row r="5" spans="1:5" ht="42" x14ac:dyDescent="0.2">
       <c r="B5" s="2" t="s">
-        <v>7</v>
+        <v>18</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>11</v>
+        <v>17</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
@@ -667,7 +664,7 @@
         <v>7</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="28" x14ac:dyDescent="0.2">
@@ -675,32 +672,40 @@
         <v>7</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="28" x14ac:dyDescent="0.2">
       <c r="C8" s="2" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="C9" s="2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="C10" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="28" x14ac:dyDescent="0.2">
       <c r="C11" s="2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="28" x14ac:dyDescent="0.2">
       <c r="C12" s="2" t="s">
-        <v>18</v>
+        <v>16</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="42" x14ac:dyDescent="0.2">
+      <c r="B13" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
13 Jul 2016:  Updated Issues Log
</commit_message>
<xml_diff>
--- a/coffeeAppIssuesLog.xlsx
+++ b/coffeeAppIssuesLog.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="18">
   <si>
     <t>Project:</t>
   </si>
@@ -35,12 +35,6 @@
     <t>ID</t>
   </si>
   <si>
-    <t>Short Desc</t>
-  </si>
-  <si>
-    <t>Long Desc</t>
-  </si>
-  <si>
     <t>Status</t>
   </si>
   <si>
@@ -50,37 +44,40 @@
     <t>Open</t>
   </si>
   <si>
-    <t>Styling</t>
-  </si>
-  <si>
-    <t>All pages need to be styled</t>
-  </si>
-  <si>
     <t>README.md</t>
   </si>
   <si>
-    <t>Public and Private Keys</t>
-  </si>
-  <si>
-    <t>Photo on home page at the bottom.</t>
-  </si>
-  <si>
-    <t>Links at the top…</t>
-  </si>
-  <si>
-    <t>Form validation</t>
-  </si>
-  <si>
-    <t>jQ-style date picker</t>
-  </si>
-  <si>
-    <t>real navigation links / hamburger</t>
-  </si>
-  <si>
-    <t>Update CB Functions / Error Handling / Front End</t>
-  </si>
-  <si>
     <t>Closed</t>
+  </si>
+  <si>
+    <t>Issue</t>
+  </si>
+  <si>
+    <t>Install Public and Private Stripe Keys</t>
+  </si>
+  <si>
+    <t>Correct placement of photo on main page.</t>
+  </si>
+  <si>
+    <t>Perform form validations.</t>
+  </si>
+  <si>
+    <t>Implement a jQ-style date-picker.</t>
+  </si>
+  <si>
+    <t>Create a proper navigation menu.</t>
+  </si>
+  <si>
+    <t>Update CB Functions / Error Handling / Back-End</t>
+  </si>
+  <si>
+    <t>Update CB Functions / Error Handling / Front-End</t>
+  </si>
+  <si>
+    <t>Need a logout button.</t>
+  </si>
+  <si>
+    <t>Need to style the login and register pages.</t>
   </si>
 </sst>
 </file>
@@ -145,7 +142,87 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="11">
+  <dxfs count="14">
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -238,24 +315,6 @@
     </dxf>
     <dxf>
       <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <name val="Source Code Pro"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" justifyLastLine="0" shrinkToFit="0"/>
-    </dxf>
-    <dxf>
-      <font>
         <b/>
         <i val="0"/>
         <strike val="0"/>
@@ -272,46 +331,6 @@
       </font>
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="1" justifyLastLine="0" shrinkToFit="0"/>
     </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium7"/>
   <extLst>
@@ -323,14 +342,13 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A3:E35" totalsRowShown="0" headerRowDxfId="6" dataDxfId="5">
-  <autoFilter ref="A3:E35"/>
-  <tableColumns count="5">
-    <tableColumn id="1" name="ID" dataDxfId="4"/>
-    <tableColumn id="2" name="Status" dataDxfId="3"/>
-    <tableColumn id="3" name="Short Desc" dataDxfId="2"/>
-    <tableColumn id="4" name="Long Desc" dataDxfId="1"/>
-    <tableColumn id="5" name="Notes" dataDxfId="0"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A3:D33" totalsRowShown="0" headerRowDxfId="13" dataDxfId="12">
+  <autoFilter ref="A3:D33"/>
+  <tableColumns count="4">
+    <tableColumn id="1" name="ID" dataDxfId="11"/>
+    <tableColumn id="2" name="Status" dataDxfId="10"/>
+    <tableColumn id="3" name="Issue" dataDxfId="9"/>
+    <tableColumn id="5" name="Notes" dataDxfId="8"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -599,7 +617,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E13"/>
+  <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
       <selection activeCell="B14" sqref="B14"/>
@@ -607,15 +625,14 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.6640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.83203125" style="2" customWidth="1"/>
-    <col min="3" max="3" width="20.33203125" style="2" customWidth="1"/>
-    <col min="4" max="4" width="33.33203125" style="2" customWidth="1"/>
-    <col min="5" max="5" width="31.83203125" style="2" customWidth="1"/>
-    <col min="6" max="16384" width="10.83203125" style="2"/>
+    <col min="1" max="1" width="9.1640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.1640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="51" style="2" customWidth="1"/>
+    <col min="4" max="6" width="40.6640625" style="2" customWidth="1"/>
+    <col min="7" max="16384" width="10.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="42" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" ht="42" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -623,86 +640,95 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="E3" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B4" s="2" t="s">
         <v>7</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D4" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B5" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B6" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6" s="2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="42" x14ac:dyDescent="0.2">
-      <c r="B5" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B6" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C6" s="2" t="s">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B7" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C7" s="2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="28" x14ac:dyDescent="0.2">
-      <c r="B7" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="C7" s="2" t="s">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B8" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B9" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C9" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="28" x14ac:dyDescent="0.2">
-      <c r="C8" s="2" t="s">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B10" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C10" s="2" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="C9" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="C10" s="2" t="s">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B11" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C11" s="2" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="28" x14ac:dyDescent="0.2">
-      <c r="C11" s="2" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" ht="28" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="B12" s="2" t="s">
+        <v>5</v>
+      </c>
       <c r="C12" s="2" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="42" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B13" s="2" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C13" s="2" t="s">
         <v>17</v>
@@ -711,17 +737,17 @@
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <conditionalFormatting sqref="B1:B1048576">
-    <cfRule type="cellIs" dxfId="10" priority="4" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">
+      <formula>"Closed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="2" priority="2" operator="equal">
       <formula>"Open"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="9" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="3" operator="equal">
       <formula>"Closed"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="8" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="4" operator="equal">
       <formula>"Open"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="7" priority="1" operator="equal">
-      <formula>"Closed"</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
16 Jul 2016:  Major styling updates.
</commit_message>
<xml_diff>
--- a/coffeeAppIssuesLog.xlsx
+++ b/coffeeAppIssuesLog.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="18">
   <si>
     <t>Project:</t>
   </si>
@@ -47,9 +47,6 @@
     <t>README.md</t>
   </si>
   <si>
-    <t>Closed</t>
-  </si>
-  <si>
     <t>Issue</t>
   </si>
   <si>
@@ -78,6 +75,9 @@
   </si>
   <si>
     <t>Need to style the login and register pages.</t>
+  </si>
+  <si>
+    <t>All are OK except the LoginController one.</t>
   </si>
 </sst>
 </file>
@@ -620,7 +620,7 @@
   <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView tabSelected="1" showRuler="0" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0.2"/>
@@ -648,18 +648,21 @@
         <v>3</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" ht="28" x14ac:dyDescent="0.2">
       <c r="B4" s="2" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
@@ -675,7 +678,7 @@
         <v>5</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
@@ -683,7 +686,7 @@
         <v>5</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
@@ -691,7 +694,7 @@
         <v>5</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
@@ -699,7 +702,7 @@
         <v>5</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
@@ -707,7 +710,7 @@
         <v>5</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
@@ -715,7 +718,7 @@
         <v>5</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
@@ -723,7 +726,7 @@
         <v>5</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
@@ -731,7 +734,7 @@
         <v>5</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>